<commit_message>
Changed hc-05 connections from hardware to software serial
</commit_message>
<xml_diff>
--- a/Kytkennät.xlsx
+++ b/Kytkennät.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\OneDrive\Omat projektit\Quad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projektit\quadcopter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18870" windowHeight="10770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="10770"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
   <si>
     <t>MPU6050</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>(INT)MPU</t>
+  </si>
+  <si>
+    <t>Moto 1</t>
+  </si>
+  <si>
+    <t>Moto 2</t>
+  </si>
+  <si>
+    <t>Moto 3</t>
+  </si>
+  <si>
+    <t>Moto 4</t>
   </si>
 </sst>
 </file>
@@ -458,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -498,6 +510,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlinkki" xfId="1" builtinId="8"/>
@@ -781,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,6 +1098,9 @@
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D29" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="E29" s="22" t="s">
         <v>41</v>
       </c>
@@ -1099,6 +1117,9 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D31" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="E31" s="22" t="s">
         <v>42</v>
       </c>
@@ -1107,18 +1128,21 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D32" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="E32" s="22" t="s">
         <v>43</v>
       </c>
       <c r="G32" s="22"/>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E33" s="23"/>
       <c r="G33" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E34" s="22">
         <v>7</v>
       </c>
@@ -1126,7 +1150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E35" s="22">
         <v>8</v>
       </c>
@@ -1134,7 +1158,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
       <c r="E36" s="22" t="s">
         <v>44</v>
       </c>
@@ -1148,7 +1175,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E37" s="22" t="s">
         <v>45</v>
       </c>
@@ -1156,7 +1183,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E38" s="22" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +1191,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E39" s="22">
         <v>12</v>
       </c>
@@ -1172,27 +1199,27 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E40" s="22">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E41" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E42" s="22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E43" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E44" s="24" t="s">
         <v>19</v>
       </c>

</xml_diff>